<commit_message>
Added code for browserdriver issue for version
</commit_message>
<xml_diff>
--- a/Driver_USER.xlsx
+++ b/Driver_USER.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="146">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>HTMLUNIT</t>
+  </si>
+  <si>
+    <t>CHROMEHEADLESS</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -578,12 +581,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -608,6 +622,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1466,9 +1486,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1478,10 +1498,11 @@
     <col min="2" max="2" width="79.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1495,10 +1516,16 @@
         <v>4</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>90</v>
       </c>
@@ -1512,10 +1539,16 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>92</v>
       </c>
@@ -1531,8 +1564,14 @@
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>34</v>
       </c>
@@ -1546,10 +1585,16 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>36</v>
       </c>
@@ -1565,8 +1610,14 @@
       <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>35</v>
       </c>
@@ -1582,8 +1633,14 @@
       <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>37</v>
       </c>
@@ -1599,8 +1656,14 @@
       <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
@@ -1616,8 +1679,14 @@
       <c r="E8" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>39</v>
       </c>
@@ -1633,8 +1702,14 @@
       <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>91</v>
       </c>
@@ -1648,12 +1723,18 @@
         <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F10">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>